<commit_message>
change in binary data between files. No actual change
</commit_message>
<xml_diff>
--- a/data/EmissionSupply/Lit_EF.xlsx
+++ b/data/EmissionSupply/Lit_EF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\EMF33\data\EmissionSupply\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D88B9723-C2BC-49EF-8568-7B0B851B1961}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4349464F-C2A1-4426-BEC2-238DDEB86932}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3225" yWindow="4560" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{64031EF1-5B25-4115-AB5A-F6D6B2D5E016}"/>
+    <workbookView xWindow="2880" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{64031EF1-5B25-4115-AB5A-F6D6B2D5E016}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -170,6 +170,1243 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Kalt 2020</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Kalt_2020!$C$2:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58.899999999999991</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>69.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>73.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>158.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>163.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>169.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Kalt_2020!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>19.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>47.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>124.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D338-40EF-95BF-F161D56036D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Daioglou 2017</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Daioglou_2017!$D$2:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.4071210769230771E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8488129230769232E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11215397538461536</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17293562153846154</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.1996325446153833</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.555269467692298</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.729833961538461</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.507788246153851</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23.819847092307697</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.032524146153847</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24.334637861538468</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24.974785738461549</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>49.824914830769231</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>123.33811504615385</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>143.25164124615384</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>146.24017729230769</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>147.51666476923077</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>148.15301166153847</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>148.82606747846154</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>149.20029493692309</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Daioglou_2017!$A$2:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D338-40EF-95BF-F161D56036D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="255355584"/>
+        <c:axId val="291786272"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="255355584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Primary Potential (EJ/yr)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="291786272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="291786272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Emission Factor (kgCO2/GJ)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="255355584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9CDBAB0-7F4C-44CD-A588-3B776C9496AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -471,8 +1708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11F2B754-BC52-441D-A6A8-4C187A55B47C}">
   <dimension ref="A4:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,6 +1756,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -526,9 +1764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A44F8D7B-827C-4B0C-9301-FF945293EE38}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -538,7 +1774,7 @@
     <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -578,7 +1814,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="8">
-        <f t="shared" ref="D3:D23" si="0">C3-((C3-B3)*(85-30))/(85-20)</f>
+        <f t="shared" ref="D3:D22" si="0">C3-((C3-B3)*(85-30))/(85-20)</f>
         <v>5.4071210769230771E-2</v>
       </c>
     </row>
@@ -883,7 +2119,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6510C5EB-23D4-4218-B0A2-B623A5C142F2}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>